<commit_message>
sheet DRILLHOLE_LITHOLOGY complete - int test fixes
</commit_message>
<xml_diff>
--- a/profiles/gsq/scripts/geochemxl/tests/data/GeochemXL-v3.0-DRILLHOLE_LITHOLOGY_04_invalid.xlsx
+++ b/profiles/gsq/scripts/geochemxl/tests/data/GeochemXL-v3.0-DRILLHOLE_LITHOLOGY_04_invalid.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Work/gsq/gsq-geochem/profiles/gsq/scripts/geochemxl/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AA34136-E7A0-FA4A-A929-39050AB586C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B47ACC-275A-9C4C-8E22-43732EFF3557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39620" yWindow="1780" windowWidth="58720" windowHeight="23280" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20600" yWindow="3740" windowWidth="58720" windowHeight="23280" tabRatio="842" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DRILLHOLE_LITHOLOGY" sheetId="15" r:id="rId1"/>
@@ -95,10 +95,10 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="DAVIES Rhys - Personal View" guid="{853B6239-A439-411F-9927-AA08BF431DBB}" mergeInterval="0" personalView="1" xWindow="2926" yWindow="109" windowWidth="2700" windowHeight="1354" tabRatio="842" activeSheetId="9"/>
+    <customWorkbookView name="KELLY Vance - Personal View" guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-678" windowWidth="2418" windowHeight="1368" tabRatio="842" activeSheetId="1" showComments="commIndAndComment"/>
+    <customWorkbookView name="HOY Derek - Personal View" guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="917" activeSheetId="6" showComments="commIndAndComment"/>
     <customWorkbookView name="TANG Joseph - Personal View" guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1928" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="842" activeSheetId="13"/>
-    <customWorkbookView name="HOY Derek - Personal View" guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" tabRatio="917" activeSheetId="6" showComments="commIndAndComment"/>
-    <customWorkbookView name="KELLY Vance - Personal View" guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" mergeInterval="0" personalView="1" maximized="1" xWindow="2391" yWindow="-678" windowWidth="2418" windowHeight="1368" tabRatio="842" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="DAVIES Rhys - Personal View" guid="{853B6239-A439-411F-9927-AA08BF431DBB}" mergeInterval="0" personalView="1" xWindow="2926" yWindow="109" windowWidth="2700" windowHeight="1354" tabRatio="842" activeSheetId="9"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1966,7 +1966,7 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -3091,23 +3091,23 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="70">
-      <selection activeCell="A8" sqref="A8"/>
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70" topLeftCell="O1">
+      <selection activeCell="S2" sqref="S2:T8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="55">
+      <selection activeCell="E8" sqref="E8"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="80" topLeftCell="S1">
       <selection activeCell="B1" sqref="B1:AB1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="55">
-      <selection activeCell="E8" sqref="E8"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="70" topLeftCell="O1">
-      <selection activeCell="S2" sqref="S2:T8"/>
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="70">
+      <selection activeCell="A8" sqref="A8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
@@ -3117,7 +3117,7 @@
       <formula>NOT(ISERROR(SEARCH("Y",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:J17 L9:L17" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>0</formula1>
       <formula2>100</formula2>
@@ -3143,21 +3143,12 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD9:AD17" xr:uid="{00000000-0002-0000-1000-000007000000}">
       <formula1>GRAIN_SIZE</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S17" xr:uid="{00000000-0002-0000-1000-000008000000}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1000-000008000000}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>S9:S17</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5954,22 +5945,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
       <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -9640,22 +9631,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" state="hidden">
       <selection activeCell="C5" sqref="C5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -16654,22 +16645,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden">
       <selection activeCell="P9" activeCellId="1" sqref="G9 P9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -24746,22 +24737,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" hiddenColumns="1" state="hidden" topLeftCell="L1">
       <selection activeCell="Q1" activeCellId="3" sqref="A1:A65536 H1:H65536 L1:N65536 Q1:V65536"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -25284,25 +25275,25 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25729,25 +25720,25 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{03B04745-F29E-4E26-B62E-F0D2264078A4}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{DEC7CBE2-9713-4252-8444-1D6959C164AB}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" scale="75" showGridLines="0" state="hidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" scale="75" showGridLines="0" state="hidden">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25787,10 +25778,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" state="veryHidden">
+    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" state="veryHidden">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{853B6239-A439-411F-9927-AA08BF431DBB}" state="veryHidden">
+    <customSheetView guid="{9F9DAF4D-D2EF-4660-943E-0C19C13C2663}" state="veryHidden">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -25799,15 +25790,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006CE8352A0AF1CD4AB9B3521FB05BB06E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe27245e9bb914202a9dc14def4cd737">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc9fd5b5-cf46-4eda-9201-7118bc1c1603" xmlns:ns3="bcd33c6e-30cb-4633-b8ec-d716de95c77b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b8902f26a47aaca738f2017df961ee0" ns2:_="" ns3:_="">
     <xsd:import namespace="cc9fd5b5-cf46-4eda-9201-7118bc1c1603"/>
@@ -26038,6 +26020,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -26053,14 +26044,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEE68A9-1E3D-4013-A8AF-E88F960C4957}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF79EA6D-2196-4B94-BF37-7CE4AD2619E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26075,6 +26058,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CEE68A9-1E3D-4013-A8AF-E88F960C4957}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>